<commit_message>
change test/train split (test=100)
</commit_message>
<xml_diff>
--- a/results-ebm/ebm-results.xlsx
+++ b/results-ebm/ebm-results.xlsx
@@ -10,14 +10,13 @@
     <sheet name="Gender" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Caste" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="coaching" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="time" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Class_ten_education" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="twelve_education" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="medium" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Class_X_Percentage" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Class_XII_Percentage" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Father_occupation" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Mother_occupation" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Class_ten_education" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="twelve_education" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="medium" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Class_X_Percentage" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Class_XII_Percentage" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Father_occupation" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Mother_occupation" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -472,16 +471,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.05152179900630298</v>
+        <v>-0.0178163614334663</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1122997315316139</v>
+        <v>-0.1354415532343072</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.03917755553997114</v>
+        <v>0.04419580299056309</v>
       </c>
       <c r="E2" t="n">
-        <v>0.06152213271735643</v>
+        <v>0.03766384537743038</v>
       </c>
     </row>
     <row r="3">
@@ -491,16 +490,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.04528932332005665</v>
+        <v>0.01579717380434011</v>
       </c>
       <c r="C3" t="n">
-        <v>0.09871508658827352</v>
+        <v>0.120091510534419</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03443833511174882</v>
+        <v>-0.03918694531829928</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.05407993924348266</v>
+        <v>-0.03339527623465495</v>
       </c>
     </row>
   </sheetData>
@@ -509,199 +508,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Average</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Excellent</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Vg</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>BANK_OFFICIAL</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>-0.9315030777103595</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.5068456544368444</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.07993611471170438</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.1983730095510804</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>BUSINESS</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>-0.1527324402203689</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.1104143298792985</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.04420021965275248</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.02367886901710382</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>COLLEGE_TEACHER</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>-0.6413734645623688</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.5506390764429359</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.5186115113588351</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.2672636867690792</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>CULTIVATOR</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.1262653969889549</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-0.1905951453121218</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.08726298175901748</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-0.0418609898034623</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>DOCTOR</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.09570082599952054</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-0.1836911772894607</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.124476723168783</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-0.05738933297745071</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>ENGINEER</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.2081084520716988</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-0.02555685307509952</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.03920144313834383</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-0.03493790849568901</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>OTHERS</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.2163481561407878</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-0.04560802405801378</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-0.04954846461511015</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-0.01864026979810987</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>SCHOOL_TEACHER</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.1479937381400569</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-0.1418364943727324</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.2018147030368416</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-0.05488421596823807</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -744,16 +550,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.6544875584661635</v>
+        <v>-0.7276229805654599</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9583941400755367</v>
+        <v>0.246264038925953</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.62532876270517</v>
+        <v>-1.624523595965311</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3177240885142861</v>
+        <v>0.9214280234331079</v>
       </c>
     </row>
     <row r="3">
@@ -763,16 +569,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.2778774837620054</v>
+        <v>-0.5048513266941949</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2351132424535955</v>
+        <v>0.1316452812892188</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.46941482637133</v>
+        <v>-1.603845357632127</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7554896280882045</v>
+        <v>0.9415593110968651</v>
       </c>
     </row>
     <row r="4">
@@ -782,16 +588,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.4269115494108938</v>
+        <v>-0.4716525897304664</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8530354140345546</v>
+        <v>0.8861957008473945</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.090505841462967</v>
+        <v>-1.11470670210302</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2215430830604325</v>
+        <v>0.2025438075549637</v>
       </c>
     </row>
     <row r="5">
@@ -801,16 +607,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.5088952581788013</v>
+        <v>-0.3768941077432657</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3793695421881026</v>
+        <v>0.7090702631245471</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.9922082510381729</v>
+        <v>-1.011966552438618</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5053591840335375</v>
+        <v>0.2970872541063498</v>
       </c>
     </row>
     <row r="6">
@@ -820,16 +626,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.4313631248255743</v>
+        <v>-0.2185312358448047</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.2329644885254952</v>
+        <v>0.3642894971013477</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.4542109159919241</v>
+        <v>-0.5920458952175216</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6050760846208187</v>
+        <v>0.2865148388729123</v>
       </c>
     </row>
     <row r="7">
@@ -839,16 +645,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.582182444402878</v>
+        <v>-0.6979472944825136</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.5483718640215096</v>
+        <v>-0.5960419866698066</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.5980644745991148</v>
+        <v>-0.934893794332917</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9115558003897112</v>
+        <v>1.208565539486198</v>
       </c>
     </row>
     <row r="8">
@@ -858,16 +664,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.03496274127795401</v>
+        <v>0.02952048766629561</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.007536796670791726</v>
+        <v>-0.03847149773842611</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01748504362057002</v>
+        <v>0.0466204436774862</v>
       </c>
       <c r="E8" t="n">
-        <v>0.009119989070428176</v>
+        <v>0.004018905409782753</v>
       </c>
     </row>
     <row r="9">
@@ -877,16 +683,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.07258282883240127</v>
+        <v>0.07313893695974176</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02350761599957869</v>
+        <v>0.01399725327691484</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2649309978393192</v>
+        <v>0.211618763548545</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.2904189115965768</v>
+        <v>-0.2258889873095929</v>
       </c>
     </row>
     <row r="10">
@@ -896,16 +702,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.00253002028391032</v>
+        <v>0.034490168156063</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.1728134462778907</v>
+        <v>-0.08900240772675676</v>
       </c>
       <c r="D10" t="n">
-        <v>0.164377553485251</v>
+        <v>0.1516913881702974</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.01889625236874658</v>
+        <v>-0.06712910679351529</v>
       </c>
     </row>
   </sheetData>
@@ -956,16 +762,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.707890246434511</v>
+        <v>-1.522489810969786</v>
       </c>
       <c r="C2" t="n">
-        <v>0.714956333927782</v>
+        <v>0.6644244153346088</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2528661718996986</v>
+        <v>0.2638110905242167</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5094868148241504</v>
+        <v>0.3930963071412782</v>
       </c>
     </row>
     <row r="3">
@@ -975,16 +781,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7163960447244441</v>
+        <v>0.5703723243055425</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.005051494553177938</v>
+        <v>-0.02895333672400313</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2838165777692688</v>
+        <v>0.317308244566617</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3266079343506339</v>
+        <v>0.231029386343876</v>
       </c>
     </row>
     <row r="4">
@@ -994,16 +800,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.860901035368431</v>
+        <v>1.727157275414552</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.6117537981063106</v>
+        <v>-0.559106336880007</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2020999308913313</v>
+        <v>-0.1978052506118028</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.2772266939301936</v>
+        <v>-0.2987745830515177</v>
       </c>
     </row>
     <row r="5">
@@ -1013,16 +819,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.267946754798031</v>
+        <v>3.1152185312969</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.907625582740474</v>
+        <v>-1.814453376531952</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.116605456899746</v>
+        <v>-1.242878005468966</v>
       </c>
       <c r="E5" t="n">
-        <v>-1.948078644844451</v>
+        <v>-1.475927810171124</v>
       </c>
     </row>
   </sheetData>
@@ -1073,16 +879,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3063641164516703</v>
+        <v>0.37302176806933</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1908188029412068</v>
+        <v>-0.2109162911484152</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03574260080154699</v>
+        <v>0.1137948932147942</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.06061980376121735</v>
+        <v>-0.1773209788383649</v>
       </c>
     </row>
     <row r="3">
@@ -1092,16 +898,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.9055481354494569</v>
+        <v>-0.9388020756368896</v>
       </c>
       <c r="C3" t="n">
-        <v>1.069124508763735</v>
+        <v>0.8637560075195296</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.04092413158266092</v>
+        <v>0.05812622744966152</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.5731847161049831</v>
+        <v>-0.3926038731240895</v>
       </c>
     </row>
     <row r="4">
@@ -1111,16 +917,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0280372176159364</v>
+        <v>0.01237438203564128</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.08916544917502391</v>
+        <v>-0.0532136776215926</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.005916859817479959</v>
+        <v>-0.04405035513547918</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1012548006810437</v>
+        <v>0.1105683535882255</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +940,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1167,96 +973,58 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>CBSE</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.23102542284638</v>
+        <v>-0.1207888431766439</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.335241277229575</v>
+        <v>-0.05365959189744179</v>
       </c>
       <c r="D2" t="n">
-        <v>0.498153697959557</v>
+        <v>-0.07855094008245525</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6732677929924676</v>
+        <v>0.1698199718799857</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>ONE</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.01164982856256504</v>
+        <v>-0.7486511925493202</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.299709098202575</v>
+        <v>0.4020675167857131</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1379952609540974</v>
+        <v>-0.05575581210761441</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08344483735670145</v>
+        <v>0.03694317882397252</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>SEVEN</t>
+          <t>SEBA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.01493804089522668</v>
+        <v>0.1172221339569855</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.3145217371638917</v>
+        <v>0.008860369397525721</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1392157354394673</v>
+        <v>0.05087238205628844</v>
       </c>
       <c r="E4" t="n">
-        <v>0.08760467498887128</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>THREE</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>-0.006217213201379426</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-0.3065471457559978</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.002278707258580072</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.2039297433894268</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>TWO</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.05193105825455891</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.3263876876403349</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-0.0962825014474675</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-0.1193475345899695</v>
+        <v>-0.1050640523051662</v>
       </c>
     </row>
   </sheetData>
@@ -1303,58 +1071,58 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>CBSE</t>
+          <t>AHSEC</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.06649954534381176</v>
+        <v>-0.1678465912546628</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2444556122508431</v>
+        <v>-0.05065792631240576</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.06876092775853304</v>
+        <v>-0.01617150903057662</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2514684226503647</v>
+        <v>0.1336665272389183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>OTHERS</t>
+          <t>CBSE</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1.151057686732986</v>
+        <v>0.1921600301683246</v>
       </c>
       <c r="C3" t="n">
-        <v>0.671962618706605</v>
+        <v>0.04985608085337251</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.2062916808709767</v>
+        <v>0.05518859675499277</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01231231090034756</v>
+        <v>-0.1616710596207673</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>SEBA</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1197654106728329</v>
+        <v>0.8170994419673605</v>
       </c>
       <c r="C4" t="n">
-        <v>0.103935611289595</v>
+        <v>0.4928416435255089</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05634981825089955</v>
+        <v>-1.030680445130755</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.155175327645013</v>
+        <v>-0.3892782724090617</v>
       </c>
     </row>
   </sheetData>
@@ -1401,39 +1169,39 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>AHSEC</t>
+          <t>ASSAMESE</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.2503721029993966</v>
+        <v>0.7417809481682555</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.02495386453365638</v>
+        <v>0.2637815338315955</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01573489108461327</v>
+        <v>-0.08783545354791973</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1664051453005139</v>
+        <v>-0.7532915347975603</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>CBSE</t>
+          <t>ENGLISH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2757647935686597</v>
+        <v>0.0455568163917259</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01426393236733067</v>
+        <v>-0.05416500094834372</v>
       </c>
       <c r="D3" t="n">
-        <v>0.06201732458585613</v>
+        <v>-0.00391976547373472</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1925299254042654</v>
+        <v>0.05241628944331309</v>
       </c>
     </row>
     <row r="4">
@@ -1443,16 +1211,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9830791463010252</v>
+        <v>-0.9759863302469386</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4334571481892807</v>
+        <v>0.1865369534347502</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.072139958044051</v>
+        <v>0.1043850236915534</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.418717149320644</v>
+        <v>0.2428076096328021</v>
       </c>
     </row>
   </sheetData>
@@ -1466,7 +1234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1499,58 +1267,77 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>ASSAMESE</t>
+          <t>Average</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8211242185146748</v>
+        <v>-0.2710725833558689</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07421921771507681</v>
+        <v>0.4163957742273031</v>
       </c>
       <c r="D2" t="n">
-        <v>0.07879891029186017</v>
+        <v>0.06256801988654964</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.8355364889974356</v>
+        <v>-0.224182188517642</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>ENGLISH</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1399594146011158</v>
+        <v>-0.08203039965249201</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.01355713879268449</v>
+        <v>0.1095625979003029</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0354095412858212</v>
+        <v>0.01476941450493001</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05778056797475006</v>
+        <v>0.002500252151855765</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>OTHERS</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.975425887094808</v>
+        <v>0.007677152202905768</v>
       </c>
       <c r="C4" t="n">
-        <v>0.04100879434174828</v>
+        <v>0.1994193185087823</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2196054447091721</v>
+        <v>-0.05351654598344976</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3328962530979198</v>
+        <v>-0.0673207604465511</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Vg</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.4239550884900293</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.6445076300297451</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.0599040287002567</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.03601284192180274</v>
       </c>
     </row>
   </sheetData>
@@ -1601,16 +1388,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9746483706585199</v>
+        <v>-0.1173631909892116</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.530150223610558</v>
+        <v>0.4081734375564864</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1749829352414689</v>
+        <v>0.07356485366449239</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.714840739411322</v>
+        <v>-0.456965389923419</v>
       </c>
     </row>
     <row r="3">
@@ -1620,16 +1407,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1175878300803163</v>
+        <v>-0.160464320387934</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1139654752063784</v>
+        <v>0.1806052088994194</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04611508704300449</v>
+        <v>-0.05455862713781379</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01522777726107043</v>
+        <v>0.0871748819317161</v>
       </c>
     </row>
     <row r="4">
@@ -1639,16 +1426,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1507112690056965</v>
+        <v>0.3898486193242168</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02256061366358865</v>
+        <v>-0.1937842566689962</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2148290497622252</v>
+        <v>0.05003077063166095</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1119459914216455</v>
+        <v>-0.2973418706972535</v>
       </c>
     </row>
     <row r="5">
@@ -1658,16 +1445,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4323814396845272</v>
+        <v>0.209465223388588</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.4138771194671206</v>
+        <v>-0.3556688166733264</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.1758973728198528</v>
+        <v>0.09666691239817177</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05371490661460741</v>
+        <v>-0.04121591754163066</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1714,77 +1501,153 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Average</t>
+          <t>BANK_OFFICIAL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.4571266154704299</v>
+        <v>-0.6127442099210322</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7119975883996058</v>
+        <v>0.4096266884755161</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4211897588703525</v>
+        <v>-0.1544004407033456</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.764174810719684</v>
+        <v>0.1814592400730257</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>BUSINESS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1897562487005778</v>
+        <v>-0.1382937410259995</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2209214206152976</v>
+        <v>0.07911685204837351</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.08122424539544436</v>
+        <v>0.04424473682751962</v>
       </c>
       <c r="E3" t="n">
-        <v>0.141845468366973</v>
+        <v>0.01651397173452741</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>COLLEGE_TEACHER</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.393643310390337</v>
+        <v>-0.5601263269600919</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1352039458297677</v>
+        <v>0.5542456937151264</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.1070307413398789</v>
+        <v>-0.4728768016969819</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.3269039144023082</v>
+        <v>0.2193520754319982</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Vg</t>
+          <t>CULTIVATOR</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3125542228115198</v>
+        <v>-0.03927692677591278</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.6251139777128066</v>
+        <v>-0.08609944509297401</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2200436347866261</v>
+        <v>0.1984171680659208</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.1144682654934949</v>
+        <v>-0.1202511514211121</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>DOCTOR</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-0.0519431066088205</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.08834832409243598</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2043142601523672</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.1230423370853135</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>ENGINEER</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1045570764899687</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.09485025550905729</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.1191121680659469</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.004371230331547245</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>OTHERS</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1285954612013405</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.04391166265906844</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.03264572778622188</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.006601007453734625</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>SCHOOL_TEACHER</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0752611468739896</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.1814357957314347</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1151591541983272</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.04528434034438487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>